<commit_message>
Adicionei a extração do MitroTik
</commit_message>
<xml_diff>
--- a/data/ensino_links_full.xlsx
+++ b/data/ensino_links_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1141"/>
+  <dimension ref="A1:E1142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24260,17 +24260,17 @@
       </c>
       <c r="C883" t="inlineStr">
         <is>
-          <t>Curso Preparatório de Física</t>
+          <t>Academia MikroTik</t>
         </is>
       </c>
       <c r="D883" t="inlineStr">
         <is>
-          <t>António Casaca</t>
+          <t>aqui</t>
         </is>
       </c>
       <c r="E883" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/antonio-manuel-carreiras-casaca</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/50_MikroTikAcademy_EN.pdf</t>
         </is>
       </c>
     </row>
@@ -24292,12 +24292,12 @@
       </c>
       <c r="D884" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>António Casaca</t>
         </is>
       </c>
       <c r="E884" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/outros-cursos/curso-preparatorio-de-fisica</t>
+          <t>https://www.isel.pt/docentes/antonio-manuel-carreiras-casaca</t>
         </is>
       </c>
     </row>
@@ -24319,12 +24319,12 @@
       </c>
       <c r="D885" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E885" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/outros-cursos/curso-preparatorio-de-fisica</t>
         </is>
       </c>
     </row>
@@ -24346,12 +24346,12 @@
       </c>
       <c r="D886" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E886" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -24373,12 +24373,12 @@
       </c>
       <c r="D887" t="inlineStr">
         <is>
-          <t>Programa detalhado</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E887" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/outros-curso/curso-preparatorio-de-fisica-programa-detalhado</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -24400,12 +24400,12 @@
       </c>
       <c r="D888" t="inlineStr">
         <is>
-          <t>aqui</t>
+          <t>Programa detalhado</t>
         </is>
       </c>
       <c r="E888" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/DF/Plano_Curso%20Fis2024%20-%20v2.pdf</t>
+          <t>https://www.isel.pt/curso/outros-curso/curso-preparatorio-de-fisica-programa-detalhado</t>
         </is>
       </c>
     </row>
@@ -24432,7 +24432,7 @@
       </c>
       <c r="E889" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/001_imagens_isel/pdf/15471_2016.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/DF/Plano_Curso%20Fis2024%20-%20v2.pdf</t>
         </is>
       </c>
     </row>
@@ -24449,17 +24449,17 @@
       </c>
       <c r="C890" t="inlineStr">
         <is>
-          <t>Curso Preparatório de Matemática</t>
+          <t>Curso Preparatório de Física</t>
         </is>
       </c>
       <c r="D890" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>aqui</t>
         </is>
       </c>
       <c r="E890" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/outros-cursos/curso-preparatorio-de-matematica</t>
+          <t>https://www.isel.pt/sites/default/files/001_imagens_isel/pdf/15471_2016.pdf</t>
         </is>
       </c>
     </row>
@@ -24481,12 +24481,12 @@
       </c>
       <c r="D891" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E891" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/outros-cursos/curso-preparatorio-de-matematica</t>
         </is>
       </c>
     </row>
@@ -24508,12 +24508,12 @@
       </c>
       <c r="D892" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E892" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -24535,12 +24535,12 @@
       </c>
       <c r="D893" t="inlineStr">
         <is>
-          <t>José Rodrigues</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E893" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/jose-alberto-de-sousa-rodrigues</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -24562,12 +24562,12 @@
       </c>
       <c r="D894" t="inlineStr">
         <is>
-          <t>Programa detalhado</t>
+          <t>José Rodrigues</t>
         </is>
       </c>
       <c r="E894" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/outros-cursos/curso-preparatorio-de-matematica-programa-detalhado</t>
+          <t>https://www.isel.pt/docentes/jose-alberto-de-sousa-rodrigues</t>
         </is>
       </c>
     </row>
@@ -24584,17 +24584,17 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>Formação de Analistas Químicos</t>
+          <t>Curso Preparatório de Matemática</t>
         </is>
       </c>
       <c r="D895" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>Programa detalhado</t>
         </is>
       </c>
       <c r="E895" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/outros-cursos/formacao-de-analistas-quimicos</t>
+          <t>https://www.isel.pt/curso/outros-cursos/curso-preparatorio-de-matematica-programa-detalhado</t>
         </is>
       </c>
     </row>
@@ -24616,12 +24616,12 @@
       </c>
       <c r="D896" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E896" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/outros-cursos/formacao-de-analistas-quimicos</t>
         </is>
       </c>
     </row>
@@ -24643,12 +24643,12 @@
       </c>
       <c r="D897" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E897" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -24670,12 +24670,12 @@
       </c>
       <c r="D898" t="inlineStr">
         <is>
-          <t>Programa e Avaliação</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E898" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/outros-cursos/formacao-de-analistas-quimicos/programa-e-avaliacao</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -24687,22 +24687,22 @@
       </c>
       <c r="B899" t="inlineStr">
         <is>
-          <t>Pós-Graduações</t>
+          <t>Outros Cursos</t>
         </is>
       </c>
       <c r="C899" t="inlineStr">
         <is>
-          <t>Conservação e Reabilitação de Construções</t>
+          <t>Formação de Analistas Químicos</t>
         </is>
       </c>
       <c r="D899" t="inlineStr">
         <is>
-          <t>Ana Rita Gião</t>
+          <t>Programa e Avaliação</t>
         </is>
       </c>
       <c r="E899" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ana-rita-faria-conceicao-de-sousa-giao</t>
+          <t>https://www.isel.pt/curso/outros-cursos/formacao-de-analistas-quimicos/programa-e-avaliacao</t>
         </is>
       </c>
     </row>
@@ -24724,12 +24724,12 @@
       </c>
       <c r="D900" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>Ana Rita Gião</t>
         </is>
       </c>
       <c r="E900" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-conservacao-e-reabilitacao-de-construcoes</t>
+          <t>https://www.isel.pt/docentes/ana-rita-faria-conceicao-de-sousa-giao</t>
         </is>
       </c>
     </row>
@@ -24751,12 +24751,12 @@
       </c>
       <c r="D901" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E901" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-conservacao-e-reabilitacao-de-construcoes/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-conservacao-e-reabilitacao-de-construcoes</t>
         </is>
       </c>
     </row>
@@ -24778,12 +24778,12 @@
       </c>
       <c r="D902" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E902" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-conservacao-e-reabilitacao-de-construcoes/candidaturas</t>
         </is>
       </c>
     </row>
@@ -24805,12 +24805,12 @@
       </c>
       <c r="D903" t="inlineStr">
         <is>
-          <t>Cristina Borges Azevedo</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E903" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ana-cristina-gaminha-ribeiro-borges-de-azevedo</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -24832,12 +24832,12 @@
       </c>
       <c r="D904" t="inlineStr">
         <is>
-          <t>Disponível aqui</t>
+          <t>Cristina Borges Azevedo</t>
         </is>
       </c>
       <c r="E904" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_CRC/13%C2%AA.%20EsquemaAulas.pdf</t>
+          <t>https://www.isel.pt/docentes/ana-cristina-gaminha-ribeiro-borges-de-azevedo</t>
         </is>
       </c>
     </row>
@@ -24859,12 +24859,12 @@
       </c>
       <c r="D905" t="inlineStr">
         <is>
-          <t>Dulce Henriques</t>
+          <t>Disponível aqui</t>
         </is>
       </c>
       <c r="E905" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-dulce-e-silva-franco-henriques</t>
+          <t>https://www.isel.pt/sites/default/files/PG_CRC/13%C2%AA.%20EsquemaAulas.pdf</t>
         </is>
       </c>
     </row>
@@ -24886,12 +24886,12 @@
       </c>
       <c r="D906" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Dulce Henriques</t>
         </is>
       </c>
       <c r="E906" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/docentes/maria-dulce-e-silva-franco-henriques</t>
         </is>
       </c>
     </row>
@@ -24913,12 +24913,12 @@
       </c>
       <c r="D907" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E907" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -24940,12 +24940,12 @@
       </c>
       <c r="D908" t="inlineStr">
         <is>
-          <t>Plano de Estudos</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E908" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/38154/plano-de-estudos</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -24967,12 +24967,12 @@
       </c>
       <c r="D909" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="E909" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/38154/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -24994,12 +24994,12 @@
       </c>
       <c r="D910" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E910" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -25021,12 +25021,12 @@
       </c>
       <c r="D911" t="inlineStr">
         <is>
-          <t>aqui</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E911" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/bolsas-next-level-impulso-adultos</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -25048,12 +25048,12 @@
       </c>
       <c r="D912" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>aqui</t>
         </is>
       </c>
       <c r="E912" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGCRC.pdf</t>
+          <t>https://www.isel.pt/comunidade/estudantes/bolsas-next-level-impulso-adultos</t>
         </is>
       </c>
     </row>
@@ -25075,12 +25075,12 @@
       </c>
       <c r="D913" t="inlineStr">
         <is>
-          <t>propina</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E913" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGCRC.pdf</t>
         </is>
       </c>
     </row>
@@ -25097,17 +25097,17 @@
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>Eficiência Energética e Sustentabilidade em Edifícios</t>
+          <t>Conservação e Reabilitação de Construções</t>
         </is>
       </c>
       <c r="D914" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>propina</t>
         </is>
       </c>
       <c r="E914" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-eficiencia-energetica-e-sustentabilidade-em-edificios</t>
+          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
         </is>
       </c>
     </row>
@@ -25129,12 +25129,12 @@
       </c>
       <c r="D915" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E915" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-eficiencia-energetica-e-sustentabilidade-em-edificios/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-eficiencia-energetica-e-sustentabilidade-em-edificios</t>
         </is>
       </c>
     </row>
@@ -25156,12 +25156,12 @@
       </c>
       <c r="D916" t="inlineStr">
         <is>
-          <t>Cláudia Casaca</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E916" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/claudia-sofia-seneca-da-luz-casaca</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-eficiencia-energetica-e-sustentabilidade-em-edificios/candidaturas</t>
         </is>
       </c>
     </row>
@@ -25183,12 +25183,12 @@
       </c>
       <c r="D917" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Cláudia Casaca</t>
         </is>
       </c>
       <c r="E917" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/docentes/claudia-sofia-seneca-da-luz-casaca</t>
         </is>
       </c>
     </row>
@@ -25210,12 +25210,12 @@
       </c>
       <c r="D918" t="inlineStr">
         <is>
-          <t>Despacho nº 8933/2022, de 20 de julho – Homologação do curso de pós-graduação em Eficiência Energética e Sustentabilidade em Edifícios</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E918" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_EESE/Despacho%208933_2022.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -25237,12 +25237,12 @@
       </c>
       <c r="D919" t="inlineStr">
         <is>
-          <t>Gonçalo Duarte</t>
+          <t>Despacho nº 8933/2022, de 20 de julho – Homologação do curso de pós-graduação em Eficiência Energética e Sustentabilidade em Edifícios</t>
         </is>
       </c>
       <c r="E919" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/goncalo-nuno-de-oliveira-duarte</t>
+          <t>https://www.isel.pt/sites/default/files/PG_EESE/Despacho%208933_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -25264,12 +25264,12 @@
       </c>
       <c r="D920" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Gonçalo Duarte</t>
         </is>
       </c>
       <c r="E920" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/docentes/goncalo-nuno-de-oliveira-duarte</t>
         </is>
       </c>
     </row>
@@ -25291,12 +25291,12 @@
       </c>
       <c r="D921" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E921" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -25318,12 +25318,12 @@
       </c>
       <c r="D922" t="inlineStr">
         <is>
-          <t>Nuno Henriques</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E922" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-paulo-ferreira-henriques</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -25345,12 +25345,12 @@
       </c>
       <c r="D923" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Nuno Henriques</t>
         </is>
       </c>
       <c r="E923" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39616/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/nuno-paulo-ferreira-henriques</t>
         </is>
       </c>
     </row>
@@ -25372,12 +25372,12 @@
       </c>
       <c r="D924" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E924" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39616/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -25399,12 +25399,12 @@
       </c>
       <c r="D925" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E925" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -25426,12 +25426,12 @@
       </c>
       <c r="D926" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E926" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEESE.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -25448,17 +25448,17 @@
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>Engenharia Optoeletrónica e Fotónica</t>
+          <t>Eficiência Energética e Sustentabilidade em Edifícios</t>
         </is>
       </c>
       <c r="D927" t="inlineStr">
         <is>
-          <t>Alessandro Fantoni</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E927" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/alessandro-fantoni</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEESE.pdf</t>
         </is>
       </c>
     </row>
@@ -25480,12 +25480,12 @@
       </c>
       <c r="D928" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>Alessandro Fantoni</t>
         </is>
       </c>
       <c r="E928" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-optoeletronica-e-fotonica</t>
+          <t>https://www.isel.pt/docentes/alessandro-fantoni</t>
         </is>
       </c>
     </row>
@@ -25507,12 +25507,12 @@
       </c>
       <c r="D929" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E929" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-optoeletronica-e-fotonica/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-optoeletronica-e-fotonica</t>
         </is>
       </c>
     </row>
@@ -25534,12 +25534,12 @@
       </c>
       <c r="D930" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E930" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-optoeletronica-e-fotonica/candidaturas</t>
         </is>
       </c>
     </row>
@@ -25561,12 +25561,12 @@
       </c>
       <c r="D931" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E931" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -25588,12 +25588,12 @@
       </c>
       <c r="D932" t="inlineStr">
         <is>
-          <t>Luís Fernandes</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E932" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luis-miguel-tavares-fernandes</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -25615,12 +25615,12 @@
       </c>
       <c r="D933" t="inlineStr">
         <is>
-          <t>Paula Louro</t>
+          <t>Luís Fernandes</t>
         </is>
       </c>
       <c r="E933" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/paula-maria-garcia-louro</t>
+          <t>https://www.isel.pt/docentes/luis-miguel-tavares-fernandes</t>
         </is>
       </c>
     </row>
@@ -25642,12 +25642,12 @@
       </c>
       <c r="D934" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Paula Louro</t>
         </is>
       </c>
       <c r="E934" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39476/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/paula-maria-garcia-louro</t>
         </is>
       </c>
     </row>
@@ -25669,12 +25669,12 @@
       </c>
       <c r="D935" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E935" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39476/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -25696,12 +25696,12 @@
       </c>
       <c r="D936" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E936" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -25723,12 +25723,12 @@
       </c>
       <c r="D937" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E937" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGOPE.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -25745,17 +25745,17 @@
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>Engenharia e Gestão de Energias Renováveis</t>
+          <t>Engenharia Optoeletrónica e Fotónica</t>
         </is>
       </c>
       <c r="D938" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E938" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-e-gestao-de-energias-renovaveis</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGOPE.pdf</t>
         </is>
       </c>
     </row>
@@ -25777,12 +25777,12 @@
       </c>
       <c r="D939" t="inlineStr">
         <is>
-          <t>Calendário de aulas 2025/2026</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E939" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_EGER/Calend%C3%A1rio%20EGER%2025_26.pdf</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-e-gestao-de-energias-renovaveis</t>
         </is>
       </c>
     </row>
@@ -25804,12 +25804,12 @@
       </c>
       <c r="D940" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Calendário de aulas 2025/2026</t>
         </is>
       </c>
       <c r="E940" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-e-gestao-de-energias-renovaveis/candidaturas</t>
+          <t>https://www.isel.pt/sites/default/files/PG_EGER/Calend%C3%A1rio%20EGER%2025_26.pdf</t>
         </is>
       </c>
     </row>
@@ -25831,12 +25831,12 @@
       </c>
       <c r="D941" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E941" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-engenharia-e-gestao-de-energias-renovaveis/candidaturas</t>
         </is>
       </c>
     </row>
@@ -25858,12 +25858,12 @@
       </c>
       <c r="D942" t="inlineStr">
         <is>
-          <t>Cristina Camus</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E942" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/cristina-ines-camus</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -25885,12 +25885,12 @@
       </c>
       <c r="D943" t="inlineStr">
         <is>
-          <t>Filipe Barata</t>
+          <t>Cristina Camus</t>
         </is>
       </c>
       <c r="E943" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/filipe-andre-de-sousa-figueira-barata</t>
+          <t>https://www.isel.pt/docentes/cristina-ines-camus</t>
         </is>
       </c>
     </row>
@@ -25912,12 +25912,12 @@
       </c>
       <c r="D944" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Filipe Barata</t>
         </is>
       </c>
       <c r="E944" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/docentes/filipe-andre-de-sousa-figueira-barata</t>
         </is>
       </c>
     </row>
@@ -25939,12 +25939,12 @@
       </c>
       <c r="D945" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E945" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -25966,12 +25966,12 @@
       </c>
       <c r="D946" t="inlineStr">
         <is>
-          <t>João Lagarto</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E946" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/joao-herminio-ninitas-lagarto</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -25993,12 +25993,12 @@
       </c>
       <c r="D947" t="inlineStr">
         <is>
-          <t>Plano de Estudos</t>
+          <t>João Lagarto</t>
         </is>
       </c>
       <c r="E947" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/10532/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/joao-herminio-ninitas-lagarto</t>
         </is>
       </c>
     </row>
@@ -26020,12 +26020,12 @@
       </c>
       <c r="D948" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="E948" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/10532/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -26047,12 +26047,12 @@
       </c>
       <c r="D949" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E949" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -26074,12 +26074,12 @@
       </c>
       <c r="D950" t="inlineStr">
         <is>
-          <t>Testemunhos</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E950" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao-em-engenharia-e-gestao-de-energias-renovaveis/testemunhos</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -26101,12 +26101,12 @@
       </c>
       <c r="D951" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Testemunhos</t>
         </is>
       </c>
       <c r="E951" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEGER.pdf</t>
+          <t>https://www.isel.pt/curso/pos-graduacao-em-engenharia-e-gestao-de-energias-renovaveis/testemunhos</t>
         </is>
       </c>
     </row>
@@ -26128,12 +26128,12 @@
       </c>
       <c r="D952" t="inlineStr">
         <is>
-          <t>propina</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E952" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEGER.pdf</t>
         </is>
       </c>
     </row>
@@ -26150,17 +26150,17 @@
       </c>
       <c r="C953" t="inlineStr">
         <is>
-          <t>Engenharia e Gestão de Risco de Desastres</t>
+          <t>Engenharia e Gestão de Energias Renováveis</t>
         </is>
       </c>
       <c r="D953" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>propina</t>
         </is>
       </c>
       <c r="E953" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-engenharia_e_gestao_do_risco_de_desastres</t>
+          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
         </is>
       </c>
     </row>
@@ -26182,12 +26182,12 @@
       </c>
       <c r="D954" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E954" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-engenharia_e_gestao_do_risco_de_desastres/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-engenharia_e_gestao_do_risco_de_desastres</t>
         </is>
       </c>
     </row>
@@ -26209,12 +26209,12 @@
       </c>
       <c r="D955" t="inlineStr">
         <is>
-          <t>Carla Costa</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E955" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/carla-maria-duarte-da-silva-e-costa</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-engenharia_e_gestao_do_risco_de_desastres/candidaturas</t>
         </is>
       </c>
     </row>
@@ -26236,12 +26236,12 @@
       </c>
       <c r="D956" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Carla Costa</t>
         </is>
       </c>
       <c r="E956" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/docentes/carla-maria-duarte-da-silva-e-costa</t>
         </is>
       </c>
     </row>
@@ -26263,12 +26263,12 @@
       </c>
       <c r="D957" t="inlineStr">
         <is>
-          <t>Despacho n.º 5379/2024</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E957" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_EGRD/Despacho5379_2024_PG%20EGRD.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -26290,12 +26290,12 @@
       </c>
       <c r="D958" t="inlineStr">
         <is>
-          <t>Duarte Caldeira</t>
+          <t>Despacho n.º 5379/2024</t>
         </is>
       </c>
       <c r="E958" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docente/duarte-caldeira</t>
+          <t>https://www.isel.pt/sites/default/files/PG_EGRD/Despacho5379_2024_PG%20EGRD.pdf</t>
         </is>
       </c>
     </row>
@@ -26317,12 +26317,12 @@
       </c>
       <c r="D959" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Duarte Caldeira</t>
         </is>
       </c>
       <c r="E959" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/docente/duarte-caldeira</t>
         </is>
       </c>
     </row>
@@ -26344,12 +26344,12 @@
       </c>
       <c r="D960" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E960" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -26371,12 +26371,12 @@
       </c>
       <c r="D961" t="inlineStr">
         <is>
-          <t>José Nascimento</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E961" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/jose-manuel-peixoto-nascimento</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -26398,12 +26398,12 @@
       </c>
       <c r="D962" t="inlineStr">
         <is>
-          <t>Maria Ana Baptista</t>
+          <t>José Nascimento</t>
         </is>
       </c>
       <c r="E962" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-ana-carvalho-viana-baptista</t>
+          <t>https://www.isel.pt/docentes/jose-manuel-peixoto-nascimento</t>
         </is>
       </c>
     </row>
@@ -26425,12 +26425,12 @@
       </c>
       <c r="D963" t="inlineStr">
         <is>
-          <t>Pedro Silva</t>
+          <t>Maria Ana Baptista</t>
         </is>
       </c>
       <c r="E963" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-manuel-fernandes-carvalho-da-silva</t>
+          <t>https://www.isel.pt/docentes/maria-ana-carvalho-viana-baptista</t>
         </is>
       </c>
     </row>
@@ -26452,12 +26452,12 @@
       </c>
       <c r="D964" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Pedro Silva</t>
         </is>
       </c>
       <c r="E964" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/40413/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/pedro-manuel-fernandes-carvalho-da-silva</t>
         </is>
       </c>
     </row>
@@ -26479,12 +26479,12 @@
       </c>
       <c r="D965" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E965" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/40413/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -26506,12 +26506,12 @@
       </c>
       <c r="D966" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E966" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -26533,12 +26533,12 @@
       </c>
       <c r="D967" t="inlineStr">
         <is>
-          <t>aqui</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E967" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEGRD.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -26560,12 +26560,12 @@
       </c>
       <c r="D968" t="inlineStr">
         <is>
-          <t>propina</t>
+          <t>aqui</t>
         </is>
       </c>
       <c r="E968" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEGRD.pdf</t>
         </is>
       </c>
     </row>
@@ -26582,17 +26582,17 @@
       </c>
       <c r="C969" t="inlineStr">
         <is>
-          <t>Especialização em Engenharia Ferroviária</t>
+          <t>Engenharia e Gestão de Risco de Desastres</t>
         </is>
       </c>
       <c r="D969" t="inlineStr">
         <is>
-          <t>Alexandra Costa</t>
+          <t>propina</t>
         </is>
       </c>
       <c r="E969" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-alexandra-cardoso-da-costa</t>
+          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
         </is>
       </c>
     </row>
@@ -26614,12 +26614,12 @@
       </c>
       <c r="D970" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>Alexandra Costa</t>
         </is>
       </c>
       <c r="E970" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-especializacao-em-engenharia-ferroviaria</t>
+          <t>https://www.isel.pt/docentes/maria-alexandra-cardoso-da-costa</t>
         </is>
       </c>
     </row>
@@ -26641,12 +26641,12 @@
       </c>
       <c r="D971" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E971" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-especializacao-em-engenharia-ferroviaria/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-especializacao-em-engenharia-ferroviaria</t>
         </is>
       </c>
     </row>
@@ -26668,12 +26668,12 @@
       </c>
       <c r="D972" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E972" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-especializacao-em-engenharia-ferroviaria/candidaturas</t>
         </is>
       </c>
     </row>
@@ -26695,12 +26695,12 @@
       </c>
       <c r="D973" t="inlineStr">
         <is>
-          <t>Despacho nº 2313/2022, de 22 de fevereiro – Homologação do curso de pós-graduação em Especialização em Engenharia Ferroviária</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E973" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/2022-02/Despacho_n_2313_2022_22_fev.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -26722,12 +26722,12 @@
       </c>
       <c r="D974" t="inlineStr">
         <is>
-          <t>Henrique Miranda</t>
+          <t>Despacho nº 2313/2022, de 22 de fevereiro – Homologação do curso de pós-graduação em Especialização em Engenharia Ferroviária</t>
         </is>
       </c>
       <c r="E974" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/henrique-manuel-borges-miranda</t>
+          <t>https://www.isel.pt/sites/default/files/2022-02/Despacho_n_2313_2022_22_fev.pdf</t>
         </is>
       </c>
     </row>
@@ -26749,12 +26749,12 @@
       </c>
       <c r="D975" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Henrique Miranda</t>
         </is>
       </c>
       <c r="E975" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/docentes/henrique-manuel-borges-miranda</t>
         </is>
       </c>
     </row>
@@ -26776,12 +26776,12 @@
       </c>
       <c r="D976" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E976" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -26803,12 +26803,12 @@
       </c>
       <c r="D977" t="inlineStr">
         <is>
-          <t>Luísa Teles Fortes</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E977" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luisa-maria-conceicao-ferreira-cardoso-teles-fortes</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -26830,12 +26830,12 @@
       </c>
       <c r="D978" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Luísa Teles Fortes</t>
         </is>
       </c>
       <c r="E978" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39431/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/luisa-maria-conceicao-ferreira-cardoso-teles-fortes</t>
         </is>
       </c>
     </row>
@@ -26857,12 +26857,12 @@
       </c>
       <c r="D979" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E979" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39431/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -26884,12 +26884,12 @@
       </c>
       <c r="D980" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E980" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -26911,12 +26911,12 @@
       </c>
       <c r="D981" t="inlineStr">
         <is>
-          <t>Testemunhos</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E981" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-especializacao-em-engenharia-ferroviaria/testemunhos</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -26938,12 +26938,12 @@
       </c>
       <c r="D982" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Testemunhos</t>
         </is>
       </c>
       <c r="E982" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEEF.pdf</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-especializacao-em-engenharia-ferroviaria/testemunhos</t>
         </is>
       </c>
     </row>
@@ -26965,12 +26965,12 @@
       </c>
       <c r="D983" t="inlineStr">
         <is>
-          <t>propina</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E983" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGEEF.pdf</t>
         </is>
       </c>
     </row>
@@ -26987,17 +26987,17 @@
       </c>
       <c r="C984" t="inlineStr">
         <is>
-          <t>Matemática para Ciência de Dados</t>
+          <t>Especialização em Engenharia Ferroviária</t>
         </is>
       </c>
       <c r="D984" t="inlineStr">
         <is>
-          <t>Ana Martins</t>
+          <t>propina</t>
         </is>
       </c>
       <c r="E984" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ana-alexandra-antunes-figueiredo-martins</t>
+          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
         </is>
       </c>
     </row>
@@ -27019,12 +27019,12 @@
       </c>
       <c r="D985" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>Ana Martins</t>
         </is>
       </c>
       <c r="E985" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-matematica-para-ciencia-de-dados</t>
+          <t>https://www.isel.pt/docentes/ana-alexandra-antunes-figueiredo-martins</t>
         </is>
       </c>
     </row>
@@ -27046,12 +27046,12 @@
       </c>
       <c r="D986" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E986" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-matematica-para-ciencia-de-dados/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-matematica-para-ciencia-de-dados</t>
         </is>
       </c>
     </row>
@@ -27073,12 +27073,12 @@
       </c>
       <c r="D987" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E987" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-matematica-para-ciencia-de-dados/candidaturas</t>
         </is>
       </c>
     </row>
@@ -27100,12 +27100,12 @@
       </c>
       <c r="D988" t="inlineStr">
         <is>
-          <t>Despacho nº 8888/2022, de 20 de julho – Homologação do curso de pós-graduação em Matemática para Ciência de Dados</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E988" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_MCD/Despacho%208888_2022.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -27127,12 +27127,12 @@
       </c>
       <c r="D989" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Despacho nº 8888/2022, de 20 de julho – Homologação do curso de pós-graduação em Matemática para Ciência de Dados</t>
         </is>
       </c>
       <c r="E989" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/sites/default/files/PG_MCD/Despacho%208888_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -27154,12 +27154,12 @@
       </c>
       <c r="D990" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E990" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -27181,12 +27181,12 @@
       </c>
       <c r="D991" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E991" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39610/plano-de-estudos</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -27208,12 +27208,12 @@
       </c>
       <c r="D992" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E992" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39610/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -27235,12 +27235,12 @@
       </c>
       <c r="D993" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E993" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -27262,12 +27262,12 @@
       </c>
       <c r="D994" t="inlineStr">
         <is>
-          <t>Sónia Carvalho</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E994" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/sonia-raquel-ferreira-carvalho</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -27289,12 +27289,12 @@
       </c>
       <c r="D995" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Sónia Carvalho</t>
         </is>
       </c>
       <c r="E995" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGMCD.pdf</t>
+          <t>https://www.isel.pt/docentes/sonia-raquel-ferreira-carvalho</t>
         </is>
       </c>
     </row>
@@ -27316,12 +27316,12 @@
       </c>
       <c r="D996" t="inlineStr">
         <is>
-          <t>propina</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E996" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGMCD.pdf</t>
         </is>
       </c>
     </row>
@@ -27338,17 +27338,17 @@
       </c>
       <c r="C997" t="inlineStr">
         <is>
-          <t>Novas Abordagens em Acústica Aplicada e Áudio</t>
+          <t>Matemática para Ciência de Dados</t>
         </is>
       </c>
       <c r="D997" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>propina</t>
         </is>
       </c>
       <c r="E997" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-novas-abordagens-em-acustica-aplicada-e-audio</t>
+          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
         </is>
       </c>
     </row>
@@ -27370,12 +27370,12 @@
       </c>
       <c r="D998" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E998" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-novas-abordagens-em-acustica-aplicada-e-audio/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-novas-abordagens-em-acustica-aplicada-e-audio</t>
         </is>
       </c>
     </row>
@@ -27397,12 +27397,12 @@
       </c>
       <c r="D999" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E999" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-novas-abordagens-em-acustica-aplicada-e-audio/candidaturas</t>
         </is>
       </c>
     </row>
@@ -27424,12 +27424,12 @@
       </c>
       <c r="D1000" t="inlineStr">
         <is>
-          <t>Despacho nº 8887/2022, de 20 de julho – Homologação do curso de pós-graduação em Novas Abordagens em Acústica Aplicada e Áudio</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E1000" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_N4A/Despacho%208887_2022.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -27451,12 +27451,12 @@
       </c>
       <c r="D1001" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Despacho nº 8887/2022, de 20 de julho – Homologação do curso de pós-graduação em Novas Abordagens em Acústica Aplicada e Áudio</t>
         </is>
       </c>
       <c r="E1001" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/sites/default/files/PG_N4A/Despacho%208887_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -27478,12 +27478,12 @@
       </c>
       <c r="D1002" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E1002" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -27505,12 +27505,12 @@
       </c>
       <c r="D1003" t="inlineStr">
         <is>
-          <t>Joel Paulo</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E1003" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/joel-vera-cruz-preto-paulo</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -27532,12 +27532,12 @@
       </c>
       <c r="D1004" t="inlineStr">
         <is>
-          <t>Paulo Trigo</t>
+          <t>Joel Paulo</t>
         </is>
       </c>
       <c r="E1004" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/paulo-manuel-trigo-candido-da-silva</t>
+          <t>https://www.isel.pt/docentes/joel-vera-cruz-preto-paulo</t>
         </is>
       </c>
     </row>
@@ -27559,12 +27559,12 @@
       </c>
       <c r="D1005" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Paulo Trigo</t>
         </is>
       </c>
       <c r="E1005" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39595/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/paulo-manuel-trigo-candido-da-silva</t>
         </is>
       </c>
     </row>
@@ -27586,12 +27586,12 @@
       </c>
       <c r="D1006" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E1006" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39595/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -27613,12 +27613,12 @@
       </c>
       <c r="D1007" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E1007" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -27640,12 +27640,12 @@
       </c>
       <c r="D1008" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E1008" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGNAAAA.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -27662,17 +27662,17 @@
       </c>
       <c r="C1009" t="inlineStr">
         <is>
-          <t>Processos Avançados de Fabrico</t>
+          <t>Novas Abordagens em Acústica Aplicada e Áudio</t>
         </is>
       </c>
       <c r="D1009" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E1009" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-processos-avancados-de-fabrico</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGNAAAA.pdf</t>
         </is>
       </c>
     </row>
@@ -27694,12 +27694,12 @@
       </c>
       <c r="D1010" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E1010" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-processos-avancados-de-fabrico/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-processos-avancados-de-fabrico</t>
         </is>
       </c>
     </row>
@@ -27721,12 +27721,12 @@
       </c>
       <c r="D1011" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E1011" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-processos-avancados-de-fabrico/candidaturas</t>
         </is>
       </c>
     </row>
@@ -27748,12 +27748,12 @@
       </c>
       <c r="D1012" t="inlineStr">
         <is>
-          <t>Despacho nº 8886/2022, de 20 de julho – Homologação do curso de pós-graduação em Processos Avançados de Fabrico</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E1012" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_PAF/Despacho%208886_2022.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -27775,12 +27775,12 @@
       </c>
       <c r="D1013" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Despacho nº 8886/2022, de 20 de julho – Homologação do curso de pós-graduação em Processos Avançados de Fabrico</t>
         </is>
       </c>
       <c r="E1013" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/sites/default/files/PG_PAF/Despacho%208886_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -27802,12 +27802,12 @@
       </c>
       <c r="D1014" t="inlineStr">
         <is>
-          <t>Ivan Galvão</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E1014" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ivan-rodolfo-pereira-garcia-de-galvao</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -27829,12 +27829,12 @@
       </c>
       <c r="D1015" t="inlineStr">
         <is>
-          <t>Ivo Bragança</t>
+          <t>Ivan Galvão</t>
         </is>
       </c>
       <c r="E1015" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ivo-manuel-ferreira-de-braganca</t>
+          <t>https://www.isel.pt/docentes/ivan-rodolfo-pereira-garcia-de-galvao</t>
         </is>
       </c>
     </row>
@@ -27856,12 +27856,12 @@
       </c>
       <c r="D1016" t="inlineStr">
         <is>
-          <t>Plano de Estudos</t>
+          <t>Ivo Bragança</t>
         </is>
       </c>
       <c r="E1016" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39639/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/ivo-manuel-ferreira-de-braganca</t>
         </is>
       </c>
     </row>
@@ -27883,12 +27883,12 @@
       </c>
       <c r="D1017" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="E1017" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39639/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -27910,12 +27910,12 @@
       </c>
       <c r="D1018" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E1018" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -27937,12 +27937,12 @@
       </c>
       <c r="D1019" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E1019" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGPAF.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -27959,17 +27959,17 @@
       </c>
       <c r="C1020" t="inlineStr">
         <is>
-          <t>Projeto e Manutenção de Instalações Elétricas</t>
+          <t>Processos Avançados de Fabrico</t>
         </is>
       </c>
       <c r="D1020" t="inlineStr">
         <is>
-          <t>António Antunes</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E1020" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/antonio-moises-ribeiro-antunes</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGPAF.pdf</t>
         </is>
       </c>
     </row>
@@ -27991,12 +27991,12 @@
       </c>
       <c r="D1021" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>António Antunes</t>
         </is>
       </c>
       <c r="E1021" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-projeto-e-manutencao-de-instalacoes-eletricas</t>
+          <t>https://www.isel.pt/docentes/antonio-moises-ribeiro-antunes</t>
         </is>
       </c>
     </row>
@@ -28018,12 +28018,12 @@
       </c>
       <c r="D1022" t="inlineStr">
         <is>
-          <t>Candidaturas</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E1022" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-projeto-e-manutencao-de-instalacoes-eletricas/candidaturas</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-projeto-e-manutencao-de-instalacoes-eletricas</t>
         </is>
       </c>
     </row>
@@ -28045,12 +28045,12 @@
       </c>
       <c r="D1023" t="inlineStr">
         <is>
-          <t>Copilot</t>
+          <t>Candidaturas</t>
         </is>
       </c>
       <c r="E1023" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
+          <t>https://www.isel.pt/curso/pos-graduacao/pos-graduacao-em-projeto-e-manutencao-de-instalacoes-eletricas/candidaturas</t>
         </is>
       </c>
     </row>
@@ -28072,12 +28072,12 @@
       </c>
       <c r="D1024" t="inlineStr">
         <is>
-          <t>Despacho nº 9366/2025, de 07 de agosto – Homologação do curso de pós-graduação em Projeto e Manutenção de Instalações Elétricas</t>
+          <t>Copilot</t>
         </is>
       </c>
       <c r="E1024" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/PG_PMIE/PG_PMIE_Despacho_9366_2025.pdf</t>
+          <t>https://www.isel.pt/eventos/apresentacao-microsoft-copilot-365</t>
         </is>
       </c>
     </row>
@@ -28099,12 +28099,12 @@
       </c>
       <c r="D1025" t="inlineStr">
         <is>
-          <t>Filipe Barata</t>
+          <t>Despacho nº 9366/2025, de 07 de agosto – Homologação do curso de pós-graduação em Projeto e Manutenção de Instalações Elétricas</t>
         </is>
       </c>
       <c r="E1025" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/filipe-andre-de-sousa-figueira-barata</t>
+          <t>https://www.isel.pt/sites/default/files/PG_PMIE/PG_PMIE_Despacho_9366_2025.pdf</t>
         </is>
       </c>
     </row>
@@ -28126,12 +28126,12 @@
       </c>
       <c r="D1026" t="inlineStr">
         <is>
-          <t>Horários do curso</t>
+          <t>Filipe Barata</t>
         </is>
       </c>
       <c r="E1026" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/docentes/filipe-andre-de-sousa-figueira-barata</t>
         </is>
       </c>
     </row>
@@ -28153,12 +28153,12 @@
       </c>
       <c r="D1027" t="inlineStr">
         <is>
-          <t>Incentivo à Investigação Exploratória</t>
+          <t>Horários do curso</t>
         </is>
       </c>
       <c r="E1027" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
@@ -28180,12 +28180,12 @@
       </c>
       <c r="D1028" t="inlineStr">
         <is>
-          <t>Luís Elvas</t>
+          <t>Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="E1028" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luis-miguel-silveiro-elvas</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
@@ -28207,12 +28207,12 @@
       </c>
       <c r="D1029" t="inlineStr">
         <is>
-          <t>Plano de estudos</t>
+          <t>Luís Elvas</t>
         </is>
       </c>
       <c r="E1029" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/39612/plano-de-estudos</t>
+          <t>https://www.isel.pt/docentes/luis-miguel-silveiro-elvas</t>
         </is>
       </c>
     </row>
@@ -28234,12 +28234,12 @@
       </c>
       <c r="D1030" t="inlineStr">
         <is>
-          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
+          <t>Plano de estudos</t>
         </is>
       </c>
       <c r="E1030" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
+          <t>https://www.isel.pt/curso/39612/plano-de-estudos</t>
         </is>
       </c>
     </row>
@@ -28261,12 +28261,12 @@
       </c>
       <c r="D1031" t="inlineStr">
         <is>
-          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento Geral dos Cursos de ​Pós-Graduação</t>
         </is>
       </c>
       <c r="E1031" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_14_02_Regulamento_Geral_dos_Cursos_de_Pos-Graduacao.pdf</t>
         </is>
       </c>
     </row>
@@ -28288,12 +28288,12 @@
       </c>
       <c r="D1032" t="inlineStr">
         <is>
-          <t>aqui.</t>
+          <t>Regulamento de Creditação de Competências do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E1032" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGPMIE.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SGAAE/Concursos_Acesso/despacho_n_4027_2022.pdf</t>
         </is>
       </c>
     </row>
@@ -28315,39 +28315,39 @@
       </c>
       <c r="D1033" t="inlineStr">
         <is>
-          <t>propina</t>
+          <t>aqui.</t>
         </is>
       </c>
       <c r="E1033" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-PGPMIE.pdf</t>
         </is>
       </c>
     </row>
     <row r="1034">
       <c r="A1034" t="inlineStr">
         <is>
-          <t>Programas de Mobilidade</t>
+          <t>Cursos</t>
         </is>
       </c>
       <c r="B1034" t="inlineStr">
         <is>
-          <t>BIP – Blended Intensive Programmes</t>
+          <t>Pós-Graduações</t>
         </is>
       </c>
       <c r="C1034" t="inlineStr">
         <is>
-          <t>BIP 2024/25</t>
+          <t>Projeto e Manutenção de Instalações Elétricas</t>
         </is>
       </c>
       <c r="D1034" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>propina</t>
         </is>
       </c>
       <c r="E1034" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip</t>
+          <t>https://www.isel.pt/sites/default/files/Despachos/2025/39_P_2025_Propinas_2025-2026.pdf</t>
         </is>
       </c>
     </row>
@@ -28369,12 +28369,12 @@
       </c>
       <c r="D1035" t="inlineStr">
         <is>
-          <t>BIP 2024/25</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E1035" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip/bip-2425</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip</t>
         </is>
       </c>
     </row>
@@ -28396,12 +28396,12 @@
       </c>
       <c r="D1036" t="inlineStr">
         <is>
-          <t>FURTHER DETAILS &gt;</t>
+          <t>BIP 2024/25</t>
         </is>
       </c>
       <c r="E1036" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip/bip-2425-speakers</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip/bip-2425</t>
         </is>
       </c>
     </row>
@@ -28423,12 +28423,12 @@
       </c>
       <c r="D1037" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>FURTHER DETAILS &gt;</t>
         </is>
       </c>
       <c r="E1037" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip/bip-2425-speakers</t>
         </is>
       </c>
     </row>
@@ -28450,12 +28450,12 @@
       </c>
       <c r="D1038" t="inlineStr">
         <is>
-          <t>physical component</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1038" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/BIP/BIP_2025-03_Detailed_Programme_Physical_Component_v4.pdf</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -28477,12 +28477,12 @@
       </c>
       <c r="D1039" t="inlineStr">
         <is>
-          <t>virtual component</t>
+          <t>physical component</t>
         </is>
       </c>
       <c r="E1039" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/BIP/3%20BIP%202025-03%20Detailed%20Description%20Virtual%20Component.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/BIP/BIP_2025-03_Detailed_Programme_Physical_Component_v4.pdf</t>
         </is>
       </c>
     </row>
@@ -28499,17 +28499,17 @@
       </c>
       <c r="C1040" t="inlineStr">
         <is>
-          <t>BIP – Blended Intensive Programmes</t>
+          <t>BIP 2024/25</t>
         </is>
       </c>
       <c r="D1040" t="inlineStr">
         <is>
-          <t>Apresentação</t>
+          <t>virtual component</t>
         </is>
       </c>
       <c r="E1040" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip</t>
+          <t>https://www.isel.pt/sites/default/files/BIP/3%20BIP%202025-03%20Detailed%20Description%20Virtual%20Component.pdf</t>
         </is>
       </c>
     </row>
@@ -28531,12 +28531,12 @@
       </c>
       <c r="D1041" t="inlineStr">
         <is>
-          <t>BIP 2024/25</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="E1041" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip/bip-2425</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip</t>
         </is>
       </c>
     </row>
@@ -28558,12 +28558,12 @@
       </c>
       <c r="D1042" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>BIP 2024/25</t>
         </is>
       </c>
       <c r="E1042" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/bip/bip-2425</t>
         </is>
       </c>
     </row>
@@ -28575,22 +28575,22 @@
       </c>
       <c r="B1043" t="inlineStr">
         <is>
-          <t>Erasmus+ Alunos Outgoing</t>
+          <t>BIP – Blended Intensive Programmes</t>
         </is>
       </c>
       <c r="C1043" t="inlineStr">
         <is>
-          <t>Erasmus+ Alunos Outgoing</t>
+          <t>BIP – Blended Intensive Programmes</t>
         </is>
       </c>
       <c r="D1043" t="inlineStr">
         <is>
-          <t>FAQ</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1043" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/faq</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -28612,12 +28612,12 @@
       </c>
       <c r="D1044" t="inlineStr">
         <is>
-          <t>Guia Erasmus+ para Estudantes Outgoing</t>
+          <t>FAQ</t>
         </is>
       </c>
       <c r="E1044" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/001_imagens_isel/pdf/Guia_ERASMUS-Plus_Outgoing_Alunos_Ver_05102024.pdf</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/faq</t>
         </is>
       </c>
     </row>
@@ -28639,12 +28639,12 @@
       </c>
       <c r="D1045" t="inlineStr">
         <is>
-          <t>Informação sobre as Bolsas Santander Mobilidade Global</t>
+          <t>Guia Erasmus+ para Estudantes Outgoing</t>
         </is>
       </c>
       <c r="E1045" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/bolsa-para-estudantes</t>
+          <t>https://www.isel.pt/sites/default/files/001_imagens_isel/pdf/Guia_ERASMUS-Plus_Outgoing_Alunos_Ver_05102024.pdf</t>
         </is>
       </c>
     </row>
@@ -28666,12 +28666,12 @@
       </c>
       <c r="D1046" t="inlineStr">
         <is>
-          <t>Informações Gerais</t>
+          <t>Informação sobre as Bolsas Santander Mobilidade Global</t>
         </is>
       </c>
       <c r="E1046" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/informacoes-gerais</t>
+          <t>https://www.isel.pt/comunidade/estudantes/bolsa-para-estudantes</t>
         </is>
       </c>
     </row>
@@ -28693,12 +28693,12 @@
       </c>
       <c r="D1047" t="inlineStr">
         <is>
-          <t>LEB – Elisabete Alegria</t>
+          <t>Informações Gerais</t>
         </is>
       </c>
       <c r="E1047" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/elisabete-clara-bastos-do-amaral-alegria</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/informacoes-gerais</t>
         </is>
       </c>
     </row>
@@ -28720,12 +28720,12 @@
       </c>
       <c r="D1048" t="inlineStr">
         <is>
-          <t>LEC – Paulo Gil Pedro</t>
+          <t>LEB – Elisabete Alegria</t>
         </is>
       </c>
       <c r="E1048" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/paulo-gil-figueiredo-tavares-pedro</t>
+          <t>https://www.isel.pt/docentes/elisabete-clara-bastos-do-amaral-alegria</t>
         </is>
       </c>
     </row>
@@ -28747,12 +28747,12 @@
       </c>
       <c r="D1049" t="inlineStr">
         <is>
-          <t>LEE – Ricardo Luís</t>
+          <t>LEC – Paulo Gil Pedro</t>
         </is>
       </c>
       <c r="E1049" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ricardo-jorge-ferreira-luis</t>
+          <t>https://www.isel.pt/docentes/paulo-gil-figueiredo-tavares-pedro</t>
         </is>
       </c>
     </row>
@@ -28774,12 +28774,12 @@
       </c>
       <c r="D1050" t="inlineStr">
         <is>
-          <t>LEETC – António Serrador</t>
+          <t>LEE – Ricardo Luís</t>
         </is>
       </c>
       <c r="E1050" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/antonio-joao-nunes-serrador</t>
+          <t>https://www.isel.pt/docentes/ricardo-jorge-ferreira-luis</t>
         </is>
       </c>
     </row>
@@ -28801,12 +28801,12 @@
       </c>
       <c r="D1051" t="inlineStr">
         <is>
-          <t>LEFA - Pedro Patrício</t>
+          <t>LEETC – António Serrador</t>
         </is>
       </c>
       <c r="E1051" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-manuel-alves-patricio-da-silva</t>
+          <t>https://www.isel.pt/docentes/antonio-joao-nunes-serrador</t>
         </is>
       </c>
     </row>
@@ -28828,12 +28828,12 @@
       </c>
       <c r="D1052" t="inlineStr">
         <is>
-          <t>LEIC – Nuno Leite</t>
+          <t>LEFA - Pedro Patrício</t>
         </is>
       </c>
       <c r="E1052" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-miguel-da-costa-de-sousa-leite</t>
+          <t>https://www.isel.pt/docentes/pedro-manuel-alves-patricio-da-silva</t>
         </is>
       </c>
     </row>
@@ -28855,12 +28855,12 @@
       </c>
       <c r="D1053" t="inlineStr">
         <is>
-          <t>LEIM – Manfred Niehus</t>
+          <t>LEIC – Nuno Leite</t>
         </is>
       </c>
       <c r="E1053" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/manfred-niehus</t>
+          <t>https://www.isel.pt/docentes/nuno-miguel-da-costa-de-sousa-leite</t>
         </is>
       </c>
     </row>
@@ -28882,12 +28882,12 @@
       </c>
       <c r="D1054" t="inlineStr">
         <is>
-          <t>LEIRT – João Ferreira Martins</t>
+          <t>LEIM – Manfred Niehus</t>
         </is>
       </c>
       <c r="E1054" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/joao-manuel-ferreira-martins</t>
+          <t>https://www.isel.pt/docentes/manfred-niehus</t>
         </is>
       </c>
     </row>
@@ -28909,12 +28909,12 @@
       </c>
       <c r="D1055" t="inlineStr">
         <is>
-          <t>LEM – Nuno Serra</t>
+          <t>LEIRT – João Ferreira Martins</t>
         </is>
       </c>
       <c r="E1055" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-ricardo-piedade-antunes-serra</t>
+          <t>https://www.isel.pt/docentes/joao-manuel-ferreira-martins</t>
         </is>
       </c>
     </row>
@@ -28936,12 +28936,12 @@
       </c>
       <c r="D1056" t="inlineStr">
         <is>
-          <t>LMATE – Cátia Dias</t>
+          <t>LEM – Nuno Serra</t>
         </is>
       </c>
       <c r="E1056" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/catia-sofia-peniche-lente-dinis-dias</t>
+          <t>https://www.isel.pt/docentes/nuno-ricardo-piedade-antunes-serra</t>
         </is>
       </c>
     </row>
@@ -28963,12 +28963,12 @@
       </c>
       <c r="D1057" t="inlineStr">
         <is>
-          <t>LTGM – Maria Teresa Santos</t>
+          <t>LMATE – Cátia Dias</t>
         </is>
       </c>
       <c r="E1057" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-teresa-loureiro-dos-santos</t>
+          <t>https://www.isel.pt/docentes/catia-sofia-peniche-lente-dinis-dias</t>
         </is>
       </c>
     </row>
@@ -28990,12 +28990,12 @@
       </c>
       <c r="D1058" t="inlineStr">
         <is>
-          <t>MEET – Alessandro Fantoni</t>
+          <t>LTGM – Maria Teresa Santos</t>
         </is>
       </c>
       <c r="E1058" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/alessandro-fantoni</t>
+          <t>https://www.isel.pt/docentes/maria-teresa-loureiro-dos-santos</t>
         </is>
       </c>
     </row>
@@ -29017,12 +29017,12 @@
       </c>
       <c r="D1059" t="inlineStr">
         <is>
-          <t>MEGI – Vítor Anes</t>
+          <t>MEET – Alessandro Fantoni</t>
         </is>
       </c>
       <c r="E1059" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/vitor-manuel-rodrigues-anes</t>
+          <t>https://www.isel.pt/docentes/alessandro-fantoni</t>
         </is>
       </c>
     </row>
@@ -29044,12 +29044,12 @@
       </c>
       <c r="D1060" t="inlineStr">
         <is>
-          <t>MEIC – Nuno Datia</t>
+          <t>MEGI – Vítor Anes</t>
         </is>
       </c>
       <c r="E1060" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-miguel-soares-datia</t>
+          <t>https://www.isel.pt/docentes/vitor-manuel-rodrigues-anes</t>
         </is>
       </c>
     </row>
@@ -29071,12 +29071,12 @@
       </c>
       <c r="D1061" t="inlineStr">
         <is>
-          <t>MEIM – Pedro Santos</t>
+          <t>MEIC – Nuno Datia</t>
         </is>
       </c>
       <c r="E1061" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docente/pedro-emanuel-albuquerque-e-baptista-dos-santos</t>
+          <t>https://www.isel.pt/docentes/nuno-miguel-soares-datia</t>
         </is>
       </c>
     </row>
@@ -29098,12 +29098,12 @@
       </c>
       <c r="D1062" t="inlineStr">
         <is>
-          <t>MEM – André Carvalho</t>
+          <t>MEIM – Pedro Santos</t>
         </is>
       </c>
       <c r="E1062" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/andre-rui-dantas-carvalho</t>
+          <t>https://www.isel.pt/docente/pedro-emanuel-albuquerque-e-baptista-dos-santos</t>
         </is>
       </c>
     </row>
@@ -29125,12 +29125,12 @@
       </c>
       <c r="D1063" t="inlineStr">
         <is>
-          <t>MEQA – Isabel João</t>
+          <t>MEM – André Carvalho</t>
         </is>
       </c>
       <c r="E1063" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/isabel-maria-da-silva-joao</t>
+          <t>https://www.isel.pt/docentes/andre-rui-dantas-carvalho</t>
         </is>
       </c>
     </row>
@@ -29152,12 +29152,12 @@
       </c>
       <c r="D1064" t="inlineStr">
         <is>
-          <t>MMAI – Teresa Melo Quinteiro</t>
+          <t>MEQA – Isabel João</t>
         </is>
       </c>
       <c r="E1064" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/teresa-maria-de-araujo-melo-quinteiro</t>
+          <t>https://www.isel.pt/docentes/isabel-maria-da-silva-joao</t>
         </is>
       </c>
     </row>
@@ -29179,12 +29179,12 @@
       </c>
       <c r="D1065" t="inlineStr">
         <is>
-          <t>Regulamento do Incentivo à Mobilidade Internacional do ISEL</t>
+          <t>MMAI – Teresa Melo Quinteiro</t>
         </is>
       </c>
       <c r="E1065" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_15_01_Regulamento_Incentivo_Mobilidade_internacional_ISEL_signed.pdf</t>
+          <t>https://www.isel.pt/docentes/teresa-maria-de-araujo-melo-quinteiro</t>
         </is>
       </c>
     </row>
@@ -29206,12 +29206,12 @@
       </c>
       <c r="D1066" t="inlineStr">
         <is>
-          <t>Regulamento para Mobilidade Académica do Instituto Superior de Engenharia de Lisboa</t>
+          <t>Regulamento do Incentivo à Mobilidade Internacional do ISEL</t>
         </is>
       </c>
       <c r="E1066" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SREI/SREI_RG_01_01%20Regulamento_Mobilidade%20Academica_ISEL_17Marco2023_signed.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_15_01_Regulamento_Incentivo_Mobilidade_internacional_ISEL_signed.pdf</t>
         </is>
       </c>
     </row>
@@ -29233,12 +29233,12 @@
       </c>
       <c r="D1067" t="inlineStr">
         <is>
-          <t>Regulamento para Mobilidade Académica no Instituto Politécnico de Lisboa</t>
+          <t>Regulamento para Mobilidade Académica do Instituto Superior de Engenharia de Lisboa</t>
         </is>
       </c>
       <c r="E1067" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SREI/03_regulamento_mobilidade_academica_IPL_DR.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SREI/SREI_RG_01_01%20Regulamento_Mobilidade%20Academica_ISEL_17Marco2023_signed.pdf</t>
         </is>
       </c>
     </row>
@@ -29260,12 +29260,12 @@
       </c>
       <c r="D1068" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Regulamento para Mobilidade Académica no Instituto Politécnico de Lisboa</t>
         </is>
       </c>
       <c r="E1068" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/sites/default/files/SREI/03_regulamento_mobilidade_academica_IPL_DR.pdf</t>
         </is>
       </c>
     </row>
@@ -29287,12 +29287,12 @@
       </c>
       <c r="D1069" t="inlineStr">
         <is>
-          <t>Testemunhos</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1069" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/testemunhos</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -29314,12 +29314,12 @@
       </c>
       <c r="D1070" t="inlineStr">
         <is>
-          <t>também podes consultar este esquema</t>
+          <t>Testemunhos</t>
         </is>
       </c>
       <c r="E1070" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/inline-images/06_Erasmus%2BOUT_QGuide_NEW_1.png</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/testemunhos</t>
         </is>
       </c>
     </row>
@@ -29336,17 +29336,17 @@
       </c>
       <c r="C1071" t="inlineStr">
         <is>
-          <t>FAQ</t>
+          <t>Erasmus+ Alunos Outgoing</t>
         </is>
       </c>
       <c r="D1071" t="inlineStr">
         <is>
-          <t>FAQ</t>
+          <t>também podes consultar este esquema</t>
         </is>
       </c>
       <c r="E1071" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/faq</t>
+          <t>https://www.isel.pt/sites/default/files/inline-images/06_Erasmus%2BOUT_QGuide_NEW_1.png</t>
         </is>
       </c>
     </row>
@@ -29368,12 +29368,12 @@
       </c>
       <c r="D1072" t="inlineStr">
         <is>
-          <t>Informações Gerais</t>
+          <t>FAQ</t>
         </is>
       </c>
       <c r="E1072" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/informacoes-gerais</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/faq</t>
         </is>
       </c>
     </row>
@@ -29395,12 +29395,12 @@
       </c>
       <c r="D1073" t="inlineStr">
         <is>
-          <t>LEB – Manuel Matos</t>
+          <t>Informações Gerais</t>
         </is>
       </c>
       <c r="E1073" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/manuel-jose-de-matos</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/informacoes-gerais</t>
         </is>
       </c>
     </row>
@@ -29422,12 +29422,12 @@
       </c>
       <c r="D1074" t="inlineStr">
         <is>
-          <t>LEC – Paulo Gil Pedro</t>
+          <t>LEB – Manuel Matos</t>
         </is>
       </c>
       <c r="E1074" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/paulo-gil-figueiredo-tavares-pedro</t>
+          <t>https://www.isel.pt/docentes/manuel-jose-de-matos</t>
         </is>
       </c>
     </row>
@@ -29449,12 +29449,12 @@
       </c>
       <c r="D1075" t="inlineStr">
         <is>
-          <t>LEE – Ricardo Luís</t>
+          <t>LEC – Paulo Gil Pedro</t>
         </is>
       </c>
       <c r="E1075" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ricardo-jorge-ferreira-luis</t>
+          <t>https://www.isel.pt/docentes/paulo-gil-figueiredo-tavares-pedro</t>
         </is>
       </c>
     </row>
@@ -29476,12 +29476,12 @@
       </c>
       <c r="D1076" t="inlineStr">
         <is>
-          <t>LEETC – António Serrador</t>
+          <t>LEE – Ricardo Luís</t>
         </is>
       </c>
       <c r="E1076" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/antonio-joao-nunes-serrador</t>
+          <t>https://www.isel.pt/docentes/ricardo-jorge-ferreira-luis</t>
         </is>
       </c>
     </row>
@@ -29503,12 +29503,12 @@
       </c>
       <c r="D1077" t="inlineStr">
         <is>
-          <t>LEFA - Pedro Patrício</t>
+          <t>LEETC – António Serrador</t>
         </is>
       </c>
       <c r="E1077" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-manuel-alves-patricio-da-silva</t>
+          <t>https://www.isel.pt/docentes/antonio-joao-nunes-serrador</t>
         </is>
       </c>
     </row>
@@ -29530,12 +29530,12 @@
       </c>
       <c r="D1078" t="inlineStr">
         <is>
-          <t>LEIC – Nuno Leite</t>
+          <t>LEFA - Pedro Patrício</t>
         </is>
       </c>
       <c r="E1078" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-miguel-da-costa-de-sousa-leite</t>
+          <t>https://www.isel.pt/docentes/pedro-manuel-alves-patricio-da-silva</t>
         </is>
       </c>
     </row>
@@ -29557,12 +29557,12 @@
       </c>
       <c r="D1079" t="inlineStr">
         <is>
-          <t>LEIM – Manfred Niehus</t>
+          <t>LEIC – Nuno Leite</t>
         </is>
       </c>
       <c r="E1079" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/manfred-niehus</t>
+          <t>https://www.isel.pt/docentes/nuno-miguel-da-costa-de-sousa-leite</t>
         </is>
       </c>
     </row>
@@ -29584,12 +29584,12 @@
       </c>
       <c r="D1080" t="inlineStr">
         <is>
-          <t>LEIRT – João Ferreira Martins</t>
+          <t>LEIM – Manfred Niehus</t>
         </is>
       </c>
       <c r="E1080" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/joao-manuel-ferreira-martins</t>
+          <t>https://www.isel.pt/docentes/manfred-niehus</t>
         </is>
       </c>
     </row>
@@ -29611,12 +29611,12 @@
       </c>
       <c r="D1081" t="inlineStr">
         <is>
-          <t>LEM – Nuno Serra</t>
+          <t>LEIRT – João Ferreira Martins</t>
         </is>
       </c>
       <c r="E1081" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-ricardo-piedade-antunes-serra</t>
+          <t>https://www.isel.pt/docentes/joao-manuel-ferreira-martins</t>
         </is>
       </c>
     </row>
@@ -29638,12 +29638,12 @@
       </c>
       <c r="D1082" t="inlineStr">
         <is>
-          <t>LEQB – Elisabete Alegria</t>
+          <t>LEM – Nuno Serra</t>
         </is>
       </c>
       <c r="E1082" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/elisabete-clara-bastos-do-amaral-alegria</t>
+          <t>https://www.isel.pt/docentes/nuno-ricardo-piedade-antunes-serra</t>
         </is>
       </c>
     </row>
@@ -29665,12 +29665,12 @@
       </c>
       <c r="D1083" t="inlineStr">
         <is>
-          <t>LMATE – Cátia Dias</t>
+          <t>LEQB – Elisabete Alegria</t>
         </is>
       </c>
       <c r="E1083" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/catia-sofia-peniche-lente-dinis-dias</t>
+          <t>https://www.isel.pt/docentes/elisabete-clara-bastos-do-amaral-alegria</t>
         </is>
       </c>
     </row>
@@ -29692,12 +29692,12 @@
       </c>
       <c r="D1084" t="inlineStr">
         <is>
-          <t>LTGM – Maria Teresa Santos</t>
+          <t>LMATE – Cátia Dias</t>
         </is>
       </c>
       <c r="E1084" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-teresa-loureiro-dos-santos</t>
+          <t>https://www.isel.pt/docentes/catia-sofia-peniche-lente-dinis-dias</t>
         </is>
       </c>
     </row>
@@ -29719,12 +29719,12 @@
       </c>
       <c r="D1085" t="inlineStr">
         <is>
-          <t>MEET – Alessandro Fantoni</t>
+          <t>LTGM – Maria Teresa Santos</t>
         </is>
       </c>
       <c r="E1085" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/alessandro-fantoni</t>
+          <t>https://www.isel.pt/docentes/maria-teresa-loureiro-dos-santos</t>
         </is>
       </c>
     </row>
@@ -29746,12 +29746,12 @@
       </c>
       <c r="D1086" t="inlineStr">
         <is>
-          <t>MEGI – Vítor Anes</t>
+          <t>MEET – Alessandro Fantoni</t>
         </is>
       </c>
       <c r="E1086" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/vitor-manuel-rodrigues-anes</t>
+          <t>https://www.isel.pt/docentes/alessandro-fantoni</t>
         </is>
       </c>
     </row>
@@ -29773,12 +29773,12 @@
       </c>
       <c r="D1087" t="inlineStr">
         <is>
-          <t>MEIC – Nuno Datia</t>
+          <t>MEGI – Vítor Anes</t>
         </is>
       </c>
       <c r="E1087" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-miguel-soares-datia</t>
+          <t>https://www.isel.pt/docentes/vitor-manuel-rodrigues-anes</t>
         </is>
       </c>
     </row>
@@ -29800,12 +29800,12 @@
       </c>
       <c r="D1088" t="inlineStr">
         <is>
-          <t>MEIM – Rui Jesus</t>
+          <t>MEIC – Nuno Datia</t>
         </is>
       </c>
       <c r="E1088" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/rui-manuel-feliciano-de-jesus</t>
+          <t>https://www.isel.pt/docentes/nuno-miguel-soares-datia</t>
         </is>
       </c>
     </row>
@@ -29827,12 +29827,12 @@
       </c>
       <c r="D1089" t="inlineStr">
         <is>
-          <t>MEM – André Carvalho</t>
+          <t>MEIM – Rui Jesus</t>
         </is>
       </c>
       <c r="E1089" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/andre-rui-dantas-carvalho</t>
+          <t>https://www.isel.pt/docentes/rui-manuel-feliciano-de-jesus</t>
         </is>
       </c>
     </row>
@@ -29854,12 +29854,12 @@
       </c>
       <c r="D1090" t="inlineStr">
         <is>
-          <t>MEQA – Isabel João</t>
+          <t>MEM – André Carvalho</t>
         </is>
       </c>
       <c r="E1090" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/isabel-maria-da-silva-joao</t>
+          <t>https://www.isel.pt/docentes/andre-rui-dantas-carvalho</t>
         </is>
       </c>
     </row>
@@ -29881,12 +29881,12 @@
       </c>
       <c r="D1091" t="inlineStr">
         <is>
-          <t>MMAI – Teresa Melo Quinteiro</t>
+          <t>MEQA – Isabel João</t>
         </is>
       </c>
       <c r="E1091" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/teresa-maria-de-araujo-melo-quinteiro</t>
+          <t>https://www.isel.pt/docentes/isabel-maria-da-silva-joao</t>
         </is>
       </c>
     </row>
@@ -29908,12 +29908,12 @@
       </c>
       <c r="D1092" t="inlineStr">
         <is>
-          <t>Regulamento para a Mobilidade Académica no IPL</t>
+          <t>MMAI – Teresa Melo Quinteiro</t>
         </is>
       </c>
       <c r="E1092" t="inlineStr">
         <is>
-          <t>https://static.escs.ipl.pt/old/pdfs/regulamentos/Regulamento-Mobilidade-IPL.pdf</t>
+          <t>https://www.isel.pt/docentes/teresa-maria-de-araujo-melo-quinteiro</t>
         </is>
       </c>
     </row>
@@ -29935,12 +29935,12 @@
       </c>
       <c r="D1093" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Regulamento para a Mobilidade Académica no IPL</t>
         </is>
       </c>
       <c r="E1093" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://static.escs.ipl.pt/old/pdfs/regulamentos/Regulamento-Mobilidade-IPL.pdf</t>
         </is>
       </c>
     </row>
@@ -29962,12 +29962,12 @@
       </c>
       <c r="D1094" t="inlineStr">
         <is>
-          <t>Testemunhos</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1094" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/testemunhos</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -29984,17 +29984,17 @@
       </c>
       <c r="C1095" t="inlineStr">
         <is>
+          <t>FAQ</t>
+        </is>
+      </c>
+      <c r="D1095" t="inlineStr">
+        <is>
           <t>Testemunhos</t>
         </is>
       </c>
-      <c r="D1095" t="inlineStr">
-        <is>
-          <t>FAQ</t>
-        </is>
-      </c>
       <c r="E1095" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/faq</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/testemunhos</t>
         </is>
       </c>
     </row>
@@ -30016,12 +30016,12 @@
       </c>
       <c r="D1096" t="inlineStr">
         <is>
-          <t>Informações Gerais</t>
+          <t>FAQ</t>
         </is>
       </c>
       <c r="E1096" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/informacoes-gerais</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/faq</t>
         </is>
       </c>
     </row>
@@ -30043,12 +30043,12 @@
       </c>
       <c r="D1097" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Informações Gerais</t>
         </is>
       </c>
       <c r="E1097" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/informacoes-gerais</t>
         </is>
       </c>
     </row>
@@ -30070,12 +30070,12 @@
       </c>
       <c r="D1098" t="inlineStr">
         <is>
-          <t>Testemunhos</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1098" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/testemunhos</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -30087,22 +30087,22 @@
       </c>
       <c r="B1099" t="inlineStr">
         <is>
-          <t>Erasmus+ Incoming Students</t>
+          <t>Erasmus+ Alunos Outgoing</t>
         </is>
       </c>
       <c r="C1099" t="inlineStr">
         <is>
-          <t>Cursos</t>
+          <t>Testemunhos</t>
         </is>
       </c>
       <c r="D1099" t="inlineStr">
         <is>
-          <t>Cursos</t>
+          <t>Testemunhos</t>
         </is>
       </c>
       <c r="E1099" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/os-nossos-cursos</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-outgoing/testemunhos</t>
         </is>
       </c>
     </row>
@@ -30124,12 +30124,12 @@
       </c>
       <c r="D1100" t="inlineStr">
         <is>
-          <t>Engenharia Biomédica</t>
+          <t>Cursos</t>
         </is>
       </c>
       <c r="E1100" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-biomedica</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/os-nossos-cursos</t>
         </is>
       </c>
     </row>
@@ -30156,7 +30156,7 @@
       </c>
       <c r="E1101" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-biomedica</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-biomedica</t>
         </is>
       </c>
     </row>
@@ -30178,12 +30178,12 @@
       </c>
       <c r="D1102" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="E1102" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-civil</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-biomedica</t>
         </is>
       </c>
     </row>
@@ -30210,7 +30210,7 @@
       </c>
       <c r="E1103" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-civil</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-civil</t>
         </is>
       </c>
     </row>
@@ -30232,12 +30232,12 @@
       </c>
       <c r="D1104" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="E1104" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-eletrotecnica</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-civil</t>
         </is>
       </c>
     </row>
@@ -30264,7 +30264,7 @@
       </c>
       <c r="E1105" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-eletrotecnica</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-eletrotecnica</t>
         </is>
       </c>
     </row>
@@ -30286,12 +30286,12 @@
       </c>
       <c r="D1106" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="E1106" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-eletronica-e-telecomunicacoes-e-de-computadores</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-eletrotecnica</t>
         </is>
       </c>
     </row>
@@ -30313,12 +30313,12 @@
       </c>
       <c r="D1107" t="inlineStr">
         <is>
-          <t>Engenharia Física Aplicada</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="E1107" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-fisica-aplicada</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-eletronica-e-telecomunicacoes-e-de-computadores</t>
         </is>
       </c>
     </row>
@@ -30340,12 +30340,12 @@
       </c>
       <c r="D1108" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="E1108" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-e-multimedia</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-fisica-aplicada</t>
         </is>
       </c>
     </row>
@@ -30372,7 +30372,7 @@
       </c>
       <c r="E1109" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-informatica-e-multimedia</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-e-multimedia</t>
         </is>
       </c>
     </row>
@@ -30394,12 +30394,12 @@
       </c>
       <c r="D1110" t="inlineStr">
         <is>
-          <t>Engenharia Informática e de Computadores</t>
+          <t>Engenharia Informática e Multimédia</t>
         </is>
       </c>
       <c r="E1110" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-e-de-computadores</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-informatica-e-multimedia</t>
         </is>
       </c>
     </row>
@@ -30426,7 +30426,7 @@
       </c>
       <c r="E1111" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-informatica-e-de-computadores</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-e-de-computadores</t>
         </is>
       </c>
     </row>
@@ -30448,12 +30448,12 @@
       </c>
       <c r="D1112" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Informática e de Computadores</t>
         </is>
       </c>
       <c r="E1112" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-redes-e-telecomunicacoes</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-informatica-e-de-computadores</t>
         </is>
       </c>
     </row>
@@ -30475,12 +30475,12 @@
       </c>
       <c r="D1113" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
         </is>
       </c>
       <c r="E1113" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-mecanica</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-redes-e-telecomunicacoes</t>
         </is>
       </c>
     </row>
@@ -30507,7 +30507,7 @@
       </c>
       <c r="E1114" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-mecanica</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-mecanica</t>
         </is>
       </c>
     </row>
@@ -30529,12 +30529,12 @@
       </c>
       <c r="D1115" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Mecânica</t>
         </is>
       </c>
       <c r="E1115" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-quimica-e-biologica</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-mecanica</t>
         </is>
       </c>
     </row>
@@ -30561,7 +30561,7 @@
       </c>
       <c r="E1116" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-quimica-e-biologica</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-quimica-e-biologica</t>
         </is>
       </c>
     </row>
@@ -30583,12 +30583,12 @@
       </c>
       <c r="D1117" t="inlineStr">
         <is>
-          <t>Engenharia da Qualidade e Ambiente</t>
+          <t>Engenharia Química e Biológica</t>
         </is>
       </c>
       <c r="E1117" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-da-qualidade-e-ambiente</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-quimica-e-biologica</t>
         </is>
       </c>
     </row>
@@ -30610,12 +30610,12 @@
       </c>
       <c r="D1118" t="inlineStr">
         <is>
-          <t>Engenharia de Eletrónica e Telecomunicações</t>
+          <t>Engenharia da Qualidade e Ambiente</t>
         </is>
       </c>
       <c r="E1118" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-de-eletronica-e-telecomunicacoes</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-da-qualidade-e-ambiente</t>
         </is>
       </c>
     </row>
@@ -30637,12 +30637,12 @@
       </c>
       <c r="D1119" t="inlineStr">
         <is>
-          <t>Engenharia e Gestão Industrial</t>
+          <t>Engenharia de Eletrónica e Telecomunicações</t>
         </is>
       </c>
       <c r="E1119" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-e-gestao-industrial</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-de-eletronica-e-telecomunicacoes</t>
         </is>
       </c>
     </row>
@@ -30664,12 +30664,12 @@
       </c>
       <c r="D1120" t="inlineStr">
         <is>
-          <t>Informações Gerais</t>
+          <t>Engenharia e Gestão Industrial</t>
         </is>
       </c>
       <c r="E1120" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/informacoes-gerais</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-engenharia-e-gestao-industrial</t>
         </is>
       </c>
     </row>
@@ -30691,12 +30691,12 @@
       </c>
       <c r="D1121" t="inlineStr">
         <is>
-          <t>Matemática Aplicada para a Indústria</t>
+          <t>Informações Gerais</t>
         </is>
       </c>
       <c r="E1121" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/mestrado/mestrado-em-matematica-aplicada-para-industria</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/informacoes-gerais</t>
         </is>
       </c>
     </row>
@@ -30718,12 +30718,12 @@
       </c>
       <c r="D1122" t="inlineStr">
         <is>
-          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+          <t>Matemática Aplicada para a Indústria</t>
         </is>
       </c>
       <c r="E1122" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-matematica-aplicada-tecnologia-e-empresa</t>
+          <t>https://www.isel.pt/curso/mestrado/mestrado-em-matematica-aplicada-para-industria</t>
         </is>
       </c>
     </row>
@@ -30745,12 +30745,12 @@
       </c>
       <c r="D1123" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
         </is>
       </c>
       <c r="E1123" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-matematica-aplicada-tecnologia-e-empresa</t>
         </is>
       </c>
     </row>
@@ -30772,12 +30772,12 @@
       </c>
       <c r="D1124" t="inlineStr">
         <is>
-          <t>Tecnologias e Gestão Municipal</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1124" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-tecnologias-e-gestao-municipal</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -30799,12 +30799,12 @@
       </c>
       <c r="D1125" t="inlineStr">
         <is>
-          <t>Unidades Curriculares</t>
+          <t>Tecnologias e Gestão Municipal</t>
         </is>
       </c>
       <c r="E1125" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SREI/Ofertas_ucs_incoming_EN_2024.pdf</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-tecnologias-e-gestao-municipal</t>
         </is>
       </c>
     </row>
@@ -30821,17 +30821,17 @@
       </c>
       <c r="C1126" t="inlineStr">
         <is>
-          <t>Erasmus+ Incoming Students</t>
+          <t>Cursos</t>
         </is>
       </c>
       <c r="D1126" t="inlineStr">
         <is>
-          <t>Cursos</t>
+          <t>Unidades Curriculares</t>
         </is>
       </c>
       <c r="E1126" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/os-nossos-cursos</t>
+          <t>https://www.isel.pt/sites/default/files/SREI/Ofertas_ucs_incoming_EN_2024.pdf</t>
         </is>
       </c>
     </row>
@@ -30853,12 +30853,12 @@
       </c>
       <c r="D1127" t="inlineStr">
         <is>
-          <t>Informações Gerais</t>
+          <t>Cursos</t>
         </is>
       </c>
       <c r="E1127" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/informacoes-gerais</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/os-nossos-cursos</t>
         </is>
       </c>
     </row>
@@ -30880,12 +30880,12 @@
       </c>
       <c r="D1128" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Informações Gerais</t>
         </is>
       </c>
       <c r="E1128" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-alunos-incoming/informacoes-gerais</t>
         </is>
       </c>
     </row>
@@ -30907,12 +30907,12 @@
       </c>
       <c r="D1129" t="inlineStr">
         <is>
-          <t>Unidades Curriculares</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1129" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SREI/Ofertas_ucs_incoming_EN_2024.pdf</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -30924,22 +30924,22 @@
       </c>
       <c r="B1130" t="inlineStr">
         <is>
-          <t>Erasmus+ Staff</t>
+          <t>Erasmus+ Incoming Students</t>
         </is>
       </c>
       <c r="C1130" t="inlineStr">
         <is>
-          <t>Erasmus+ Staff</t>
+          <t>Erasmus+ Incoming Students</t>
         </is>
       </c>
       <c r="D1130" t="inlineStr">
         <is>
-          <t>Guia Erasmus+ para Staff</t>
+          <t>Unidades Curriculares</t>
         </is>
       </c>
       <c r="E1130" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/SREI/Guia_ERASMUS-Plus_Staff.pdf</t>
+          <t>https://www.isel.pt/sites/default/files/SREI/Ofertas_ucs_incoming_EN_2024.pdf</t>
         </is>
       </c>
     </row>
@@ -30961,12 +30961,12 @@
       </c>
       <c r="D1131" t="inlineStr">
         <is>
-          <t>Informações Gerais</t>
+          <t>Guia Erasmus+ para Staff</t>
         </is>
       </c>
       <c r="E1131" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-staff/informacoes-gerais</t>
+          <t>https://www.isel.pt/sites/default/files/SREI/Guia_ERASMUS-Plus_Staff.pdf</t>
         </is>
       </c>
     </row>
@@ -30988,12 +30988,12 @@
       </c>
       <c r="D1132" t="inlineStr">
         <is>
-          <t>Instituições parceiras</t>
+          <t>Informações Gerais</t>
         </is>
       </c>
       <c r="E1132" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-staff/instituicoes-parceiras</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-staff/informacoes-gerais</t>
         </is>
       </c>
     </row>
@@ -31015,12 +31015,12 @@
       </c>
       <c r="D1133" t="inlineStr">
         <is>
-          <t>Regulamento do Incentivo à Mobilidade Internacional do ISEL</t>
+          <t>Instituições parceiras</t>
         </is>
       </c>
       <c r="E1133" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_15_01_Regulamento_Incentivo_Mobilidade_internacional_ISEL_signed.pdf</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/erasmus-staff/instituicoes-parceiras</t>
         </is>
       </c>
     </row>
@@ -31042,12 +31042,12 @@
       </c>
       <c r="D1134" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Regulamento do Incentivo à Mobilidade Internacional do ISEL</t>
         </is>
       </c>
       <c r="E1134" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/sites/default/files/002_pdf/PRE_RG_15_01_Regulamento_Incentivo_Mobilidade_internacional_ISEL_signed.pdf</t>
         </is>
       </c>
     </row>
@@ -31064,7 +31064,7 @@
       </c>
       <c r="C1135" t="inlineStr">
         <is>
-          <t>Instituições parceiras</t>
+          <t>Erasmus+ Staff</t>
         </is>
       </c>
       <c r="D1135" t="inlineStr">
@@ -31086,22 +31086,22 @@
       </c>
       <c r="B1136" t="inlineStr">
         <is>
-          <t>Outros Programas</t>
+          <t>Erasmus+ Staff</t>
         </is>
       </c>
       <c r="C1136" t="inlineStr">
         <is>
-          <t>Outros Programas</t>
+          <t>Instituições parceiras</t>
         </is>
       </c>
       <c r="D1136" t="inlineStr">
         <is>
-          <t>Programa Vulcanus</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1136" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programa-vulcanus</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -31123,12 +31123,12 @@
       </c>
       <c r="D1137" t="inlineStr">
         <is>
-          <t>Programas de intercâmbio</t>
+          <t>Programa Vulcanus</t>
         </is>
       </c>
       <c r="E1137" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programas-de-intercambio</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programa-vulcanus</t>
         </is>
       </c>
     </row>
@@ -31150,12 +31150,12 @@
       </c>
       <c r="D1138" t="inlineStr">
         <is>
-          <t>Sugestões, reclamações ou denúncias</t>
+          <t>Programas de intercâmbio</t>
         </is>
       </c>
       <c r="E1138" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programas-de-intercambio</t>
         </is>
       </c>
     </row>
@@ -31172,17 +31172,17 @@
       </c>
       <c r="C1139" t="inlineStr">
         <is>
-          <t>Programa Vulcanus</t>
+          <t>Outros Programas</t>
         </is>
       </c>
       <c r="D1139" t="inlineStr">
         <is>
-          <t>Programa Vulcanus</t>
+          <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
       <c r="E1139" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programa-vulcanus</t>
+          <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>
       </c>
     </row>
@@ -31204,12 +31204,12 @@
       </c>
       <c r="D1140" t="inlineStr">
         <is>
-          <t>Programas de intercâmbio</t>
+          <t>Programa Vulcanus</t>
         </is>
       </c>
       <c r="E1140" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programas-de-intercambio</t>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programa-vulcanus</t>
         </is>
       </c>
     </row>
@@ -31231,10 +31231,37 @@
       </c>
       <c r="D1141" t="inlineStr">
         <is>
+          <t>Programas de intercâmbio</t>
+        </is>
+      </c>
+      <c r="E1141" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/programas-de-mobilidade/outros-programas/informacoes-gerais/programas-de-intercambio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>Programas de Mobilidade</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Outros Programas</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>Programa Vulcanus</t>
+        </is>
+      </c>
+      <c r="D1142" t="inlineStr">
+        <is>
           <t>Sugestões, reclamações ou denúncias</t>
         </is>
       </c>
-      <c r="E1141" t="inlineStr">
+      <c r="E1142" t="inlineStr">
         <is>
           <t>https://www.isel.pt/sugestoes-reclamacoes-ou-denuncias</t>
         </is>

</xml_diff>